<commit_message>
Modify Lab 5 and Make All folder or File to be present
</commit_message>
<xml_diff>
--- a/Lab4/Lab4_663380241-1.xlsx
+++ b/Lab4/Lab4_663380241-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HomeWork\CP353201\AllLab\Lab4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\663380241-1\CP353201\Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FE6D24-6AFA-4D1A-A2A3-9FF68ACCA07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300A9479-1BCC-4A36-B70D-2600A00400D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D3B1ECF-CE0B-884D-A6E2-5EDB198A06FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{2D3B1ECF-CE0B-884D-A6E2-5EDB198A06FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Summary" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="94">
   <si>
     <t>Test Case Design and Test Results</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>Standard</t>
-  </si>
-  <si>
-    <t>Gold</t>
   </si>
   <si>
     <t>TC014</t>
@@ -321,7 +318,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -498,7 +495,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -555,6 +552,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -587,18 +602,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -939,20 +942,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CE7BA3-0BEF-0C45-955A-B350FDBEC636}">
   <dimension ref="A2:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="27.75" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="27.75"/>
   <cols>
-    <col min="1" max="1" width="33.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.125" style="1" customWidth="1"/>
-    <col min="3" max="6" width="9.125" style="1"/>
-    <col min="7" max="7" width="21.75" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="33.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" style="1" customWidth="1"/>
+    <col min="3" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="21.77734375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="55.5" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:7">
       <c r="A2" s="13" t="s">
         <v>44</v>
       </c>
@@ -975,7 +978,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
@@ -990,11 +993,11 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.65">
+      <c r="G3" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
         <v>46</v>
       </c>
@@ -1010,10 +1013,10 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.65">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="3"/>
@@ -1022,17 +1025,17 @@
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:7">
       <c r="A6" s="18" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="3">
         <v>32</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="24">
         <v>12</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="25">
         <v>20</v>
       </c>
       <c r="E6" s="3"/>
@@ -1048,34 +1051,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFEE3D1E-0814-D34A-9C7B-86FDE5AD12C8}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="27.75" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="27.75"/>
   <cols>
-    <col min="1" max="1" width="21.125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="21.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.125" style="1" customWidth="1"/>
-    <col min="8" max="10" width="10.75" style="1"/>
-    <col min="11" max="11" width="14.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" style="1" customWidth="1"/>
+    <col min="2" max="4" width="21.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" style="1" customWidth="1"/>
+    <col min="8" max="10" width="10.77734375" style="1"/>
+    <col min="11" max="11" width="14.21875" style="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.25" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.75" style="1"/>
+    <col min="13" max="13" width="15.21875" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.65">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
       <c r="J1" s="2"/>
       <c r="K1" s="8" t="s">
         <v>23</v>
@@ -1087,7 +1090,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:13">
       <c r="G2" s="4"/>
       <c r="J2" s="3" t="s">
         <v>10</v>
@@ -1102,16 +1105,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:13">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="5" t="s">
         <v>21</v>
       </c>
@@ -1131,16 +1134,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:13">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1154,25 +1157,25 @@
         <v>50000</v>
       </c>
       <c r="L4" s="21">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="M4" s="21">
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:13">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="27"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>7</v>
@@ -1181,13 +1184,13 @@
         <v>99999</v>
       </c>
       <c r="L5" s="21">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="M5" s="21">
         <v>999</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:13">
       <c r="J6" s="3" t="s">
         <v>6</v>
       </c>
@@ -1195,33 +1198,33 @@
         <v>100000</v>
       </c>
       <c r="L6" s="21">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="M6" s="21">
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:13" ht="24.95" customHeight="1">
+      <c r="A7" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31" t="s">
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="32" t="s">
+      <c r="F7" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="38" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.65">
-      <c r="A8" s="31"/>
+    <row r="8" spans="1:13">
+      <c r="A8" s="37"/>
       <c r="B8" s="8" t="s">
         <v>23</v>
       </c>
@@ -1231,11 +1234,11 @@
       <c r="D8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="32"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.65">
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="38"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="19" t="s">
         <v>49</v>
       </c>
@@ -1243,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="8">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D9" s="8">
         <v>500</v>
@@ -1258,15 +1261,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:13">
       <c r="A10" s="19" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="8">
         <v>1</v>
       </c>
-      <c r="C10" s="8">
-        <v>4</v>
+      <c r="C10" s="22">
+        <v>15</v>
       </c>
       <c r="D10" s="8">
         <v>500</v>
@@ -1281,61 +1284,61 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:13">
       <c r="A11" s="19" t="s">
         <v>51</v>
       </c>
       <c r="B11" s="8">
         <v>50000</v>
       </c>
-      <c r="C11" s="8">
-        <v>4</v>
+      <c r="C11" s="22">
+        <v>15</v>
       </c>
       <c r="D11" s="8">
         <v>500</v>
       </c>
-      <c r="E11" s="19" t="s">
-        <v>63</v>
+      <c r="E11" s="23" t="s">
+        <v>62</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:13">
       <c r="A12" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B12" s="8">
         <v>99999</v>
       </c>
-      <c r="C12" s="8">
-        <v>4</v>
+      <c r="C12" s="22">
+        <v>15</v>
       </c>
       <c r="D12" s="8">
         <v>500</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>63</v>
+      <c r="E12" s="23" t="s">
+        <v>62</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:13">
       <c r="A13" s="19" t="s">
         <v>53</v>
       </c>
       <c r="B13" s="8">
         <v>100000</v>
       </c>
-      <c r="C13" s="8">
-        <v>4</v>
+      <c r="C13" s="22">
+        <v>15</v>
       </c>
       <c r="D13" s="8">
         <v>500</v>
@@ -1344,13 +1347,13 @@
         <v>62</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:13">
       <c r="A14" s="19" t="s">
         <v>54</v>
       </c>
@@ -1373,7 +1376,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:13">
       <c r="A15" s="19" t="s">
         <v>55</v>
       </c>
@@ -1396,7 +1399,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:13">
       <c r="A16" s="19" t="s">
         <v>56</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>50000</v>
       </c>
       <c r="C16" s="3">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D16" s="8">
         <v>500</v>
@@ -1413,13 +1416,13 @@
         <v>62</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:7">
       <c r="A17" s="19" t="s">
         <v>57</v>
       </c>
@@ -1427,7 +1430,7 @@
         <v>50000</v>
       </c>
       <c r="C17" s="3">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D17" s="8">
         <v>500</v>
@@ -1436,13 +1439,13 @@
         <v>62</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G17" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
         <v>58</v>
       </c>
@@ -1450,7 +1453,7 @@
         <v>50000</v>
       </c>
       <c r="C18" s="8">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D18" s="8">
         <v>0</v>
@@ -1465,15 +1468,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
         <v>59</v>
       </c>
       <c r="B19" s="8">
         <v>50000</v>
       </c>
-      <c r="C19" s="8">
-        <v>4</v>
+      <c r="C19" s="22">
+        <v>15</v>
       </c>
       <c r="D19" s="8">
         <v>1</v>
@@ -1488,38 +1491,38 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
         <v>60</v>
       </c>
       <c r="B20" s="8">
         <v>50000</v>
       </c>
-      <c r="C20" s="8">
-        <v>4</v>
+      <c r="C20" s="22">
+        <v>15</v>
       </c>
       <c r="D20" s="3">
         <v>999</v>
       </c>
-      <c r="E20" s="19" t="s">
-        <v>63</v>
+      <c r="E20" s="23" t="s">
+        <v>62</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:7">
       <c r="A21" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B21" s="8">
         <v>50000</v>
       </c>
-      <c r="C21" s="8">
-        <v>4</v>
+      <c r="C21" s="22">
+        <v>15</v>
       </c>
       <c r="D21" s="3">
         <v>1000</v>
@@ -1528,7 +1531,7 @@
         <v>62</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>39</v>
@@ -1555,34 +1558,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A52C6A-99BA-484C-B915-27B6FC4D32AF}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="27.75" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="27.75"/>
   <cols>
-    <col min="1" max="1" width="20.375" style="1" customWidth="1"/>
-    <col min="2" max="4" width="21.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.125" style="1" customWidth="1"/>
-    <col min="8" max="10" width="10.75" style="1"/>
-    <col min="11" max="11" width="17.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="21.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.109375" style="1" customWidth="1"/>
+    <col min="8" max="10" width="10.77734375" style="1"/>
+    <col min="11" max="11" width="17.33203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="12" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.75" style="1"/>
+    <col min="13" max="13" width="17.6640625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.65">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="30"/>
       <c r="J1" s="2"/>
       <c r="K1" s="3" t="s">
         <v>23</v>
@@ -1594,7 +1597,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:13">
       <c r="G2" s="4"/>
       <c r="J2" s="3" t="s">
         <v>11</v>
@@ -1609,16 +1612,16 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:13">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
       <c r="F3" s="5" t="s">
         <v>21</v>
       </c>
@@ -1638,16 +1641,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:13">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
       <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1667,19 +1670,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:13">
       <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="27"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="F5" s="5" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>8</v>
@@ -1688,13 +1691,13 @@
         <v>50000</v>
       </c>
       <c r="L5" s="21">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="M5" s="21">
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:13">
       <c r="J6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1702,28 +1705,28 @@
         <v>99999</v>
       </c>
       <c r="L6" s="21">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="M6" s="21">
         <v>999</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:13" ht="24.95" customHeight="1">
+      <c r="A7" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31" t="s">
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="32" t="s">
+      <c r="F7" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="38" t="s">
         <v>16</v>
       </c>
       <c r="J7" s="3" t="s">
@@ -1733,14 +1736,14 @@
         <v>100000</v>
       </c>
       <c r="L7" s="21">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="M7" s="21">
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.65">
-      <c r="A8" s="31"/>
+    <row r="8" spans="1:13">
+      <c r="A8" s="37"/>
       <c r="B8" s="8" t="s">
         <v>23</v>
       </c>
@@ -1750,9 +1753,9 @@
       <c r="D8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="32"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="38"/>
       <c r="J8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1760,27 +1763,27 @@
         <v>100001</v>
       </c>
       <c r="L8" s="3">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="M8" s="3">
         <v>1001</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:13">
       <c r="A9" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" s="8">
         <v>-1</v>
       </c>
       <c r="C9" s="19">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D9" s="19">
         <v>500</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>62</v>
@@ -1789,15 +1792,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:13">
       <c r="A10" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="8">
         <v>0</v>
       </c>
-      <c r="C10" s="19">
-        <v>4</v>
+      <c r="C10" s="23">
+        <v>15</v>
       </c>
       <c r="D10" s="19">
         <v>500</v>
@@ -1812,15 +1815,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:13">
       <c r="A11" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="8">
         <v>1</v>
       </c>
-      <c r="C11" s="19">
-        <v>4</v>
+      <c r="C11" s="23">
+        <v>15</v>
       </c>
       <c r="D11" s="19">
         <v>500</v>
@@ -1835,61 +1838,61 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:13">
       <c r="A12" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="8">
         <v>50000</v>
       </c>
-      <c r="C12" s="19">
-        <v>4</v>
+      <c r="C12" s="23">
+        <v>15</v>
       </c>
       <c r="D12" s="19">
         <v>500</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>63</v>
+      <c r="E12" s="23" t="s">
+        <v>62</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:13">
       <c r="A13" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="19">
         <v>99999</v>
       </c>
-      <c r="C13" s="19">
-        <v>4</v>
+      <c r="C13" s="23">
+        <v>15</v>
       </c>
       <c r="D13" s="19">
         <v>500</v>
       </c>
-      <c r="E13" s="19" t="s">
-        <v>63</v>
+      <c r="E13" s="23" t="s">
+        <v>62</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:13">
       <c r="A14" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B14" s="19">
         <v>100000</v>
       </c>
-      <c r="C14" s="19">
-        <v>4</v>
+      <c r="C14" s="23">
+        <v>15</v>
       </c>
       <c r="D14" s="19">
         <v>500</v>
@@ -1898,21 +1901,21 @@
         <v>62</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:13">
       <c r="A15" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="8">
         <v>100001</v>
       </c>
-      <c r="C15" s="19">
-        <v>4</v>
+      <c r="C15" s="23">
+        <v>15</v>
       </c>
       <c r="D15" s="19">
         <v>500</v>
@@ -1921,15 +1924,15 @@
         <v>62</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:13">
       <c r="A16" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="19">
         <v>50000</v>
@@ -1941,7 +1944,7 @@
         <v>500</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>62</v>
@@ -1950,9 +1953,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:7">
       <c r="A17" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="19">
         <v>50000</v>
@@ -1973,9 +1976,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:7">
       <c r="A18" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="19">
         <v>50000</v>
@@ -1996,15 +1999,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:7">
       <c r="A19" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="19">
         <v>50000</v>
       </c>
       <c r="C19" s="19">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D19" s="19">
         <v>500</v>
@@ -2013,21 +2016,21 @@
         <v>62</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G19" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:7">
       <c r="A20" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" s="19">
         <v>50000</v>
       </c>
       <c r="C20" s="19">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D20" s="19">
         <v>500</v>
@@ -2036,21 +2039,21 @@
         <v>62</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:7">
       <c r="A21" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" s="19">
         <v>50000</v>
       </c>
       <c r="C21" s="8">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="D21" s="19">
         <v>500</v>
@@ -2059,27 +2062,27 @@
         <v>62</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G21" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:7">
       <c r="A22" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22" s="19">
         <v>50000</v>
       </c>
       <c r="C22" s="19">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D22" s="8">
         <v>-1</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F22" s="19" t="s">
         <v>62</v>
@@ -2088,15 +2091,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:7">
       <c r="A23" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" s="19">
         <v>50000</v>
       </c>
-      <c r="C23" s="19">
-        <v>4</v>
+      <c r="C23" s="23">
+        <v>15</v>
       </c>
       <c r="D23" s="19">
         <v>0</v>
@@ -2111,15 +2114,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:7">
       <c r="A24" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" s="19">
         <v>50000</v>
       </c>
-      <c r="C24" s="19">
-        <v>4</v>
+      <c r="C24" s="23">
+        <v>15</v>
       </c>
       <c r="D24" s="19">
         <v>1</v>
@@ -2134,38 +2137,38 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="25" spans="1:7">
       <c r="A25" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="19">
         <v>50000</v>
       </c>
-      <c r="C25" s="19">
-        <v>4</v>
+      <c r="C25" s="23">
+        <v>15</v>
       </c>
       <c r="D25" s="19">
         <v>999</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>63</v>
+      <c r="E25" s="22" t="s">
+        <v>62</v>
       </c>
       <c r="F25" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:7">
       <c r="A26" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" s="19">
         <v>50000</v>
       </c>
-      <c r="C26" s="19">
-        <v>4</v>
+      <c r="C26" s="23">
+        <v>15</v>
       </c>
       <c r="D26" s="19">
         <v>1000</v>
@@ -2174,21 +2177,21 @@
         <v>62</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:7">
       <c r="A27" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B27" s="19">
         <v>50000</v>
       </c>
-      <c r="C27" s="19">
-        <v>4</v>
+      <c r="C27" s="23">
+        <v>15</v>
       </c>
       <c r="D27" s="8">
         <v>1001</v>
@@ -2197,7 +2200,7 @@
         <v>62</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>39</v>
@@ -2224,22 +2227,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8068CBD9-38BE-794D-AE4F-17FC500CF117}">
   <dimension ref="A2:K5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="27.75" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="27.75"/>
   <cols>
-    <col min="1" max="2" width="10.75" style="1"/>
-    <col min="3" max="3" width="33.25" style="1" customWidth="1"/>
-    <col min="4" max="5" width="10.75" style="1"/>
+    <col min="1" max="2" width="10.77734375" style="1"/>
+    <col min="3" max="3" width="33.21875" style="1" customWidth="1"/>
+    <col min="4" max="5" width="10.77734375" style="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="10" width="10.75" style="1"/>
-    <col min="11" max="11" width="61.125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.75" style="1"/>
+    <col min="7" max="10" width="10.77734375" style="1"/>
+    <col min="11" max="11" width="61.109375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="55.5" x14ac:dyDescent="0.65">
+    <row r="2" spans="1:11" ht="55.5">
       <c r="A2" s="9" t="s">
         <v>26</v>
       </c>
@@ -2274,79 +2277,79 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="100.5" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:11" ht="100.5" customHeight="1">
       <c r="A3" s="11">
         <v>1</v>
       </c>
       <c r="B3" s="11">
         <v>1</v>
       </c>
-      <c r="C3" s="35" t="s">
-        <v>87</v>
+      <c r="C3" s="26" t="s">
+        <v>86</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
-      <c r="K3" s="35" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="83.25" x14ac:dyDescent="0.65">
+      <c r="K3" s="26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="55.5">
       <c r="A4" s="11">
         <v>2</v>
       </c>
       <c r="B4" s="11">
         <v>2</v>
       </c>
-      <c r="C4" s="35" t="s">
-        <v>89</v>
+      <c r="C4" s="26" t="s">
+        <v>88</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="35" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="83.25" x14ac:dyDescent="0.65">
+      <c r="K4" s="26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="83.25">
       <c r="A5" s="11">
         <v>3</v>
       </c>
       <c r="B5" s="11">
         <v>3</v>
       </c>
-      <c r="C5" s="35" t="s">
-        <v>91</v>
+      <c r="C5" s="26" t="s">
+        <v>90</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11"/>
-      <c r="K5" s="35" t="s">
-        <v>92</v>
+      <c r="K5" s="26" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>